<commit_message>
organiz imports and make it possible to switch between cloud and test servers
</commit_message>
<xml_diff>
--- a/data_sheets/test_coverage.xlsx
+++ b/data_sheets/test_coverage.xlsx
@@ -105,9 +105,6 @@
     <t xml:space="preserve">Switching from grid view to list view </t>
   </si>
   <si>
-    <t>Check if a new user can be successfully signed in</t>
-  </si>
-  <si>
     <t>test_sign_up_link</t>
   </si>
   <si>
@@ -130,6 +127,9 @@
   </si>
   <si>
     <t>Check if a user  can sign in providing valid credentials</t>
+  </si>
+  <si>
+    <t>Check if a new user can be successfully signed up</t>
   </si>
 </sst>
 </file>
@@ -506,7 +506,7 @@
   <dimension ref="A2:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,7 +557,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -634,10 +634,10 @@
         <v>21</v>
       </c>
       <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
         <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -654,10 +654,10 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
@@ -674,10 +674,10 @@
         <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -694,10 +694,10 @@
         <v>21</v>
       </c>
       <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
         <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
add filters to test_coverage.xlsx
</commit_message>
<xml_diff>
--- a/data_sheets/test_coverage.xlsx
+++ b/data_sheets/test_coverage.xlsx
@@ -15,6 +15,9 @@
     <sheet name="test_cases" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">test_cases!$A$2:$H$10</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -506,7 +509,7 @@
   <dimension ref="A2:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,6 +710,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:H10"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>

</xml_diff>

<commit_message>
updated some test cases
</commit_message>
<xml_diff>
--- a/data_sheets/test_coverage.xlsx
+++ b/data_sheets/test_coverage.xlsx
@@ -84,9 +84,6 @@
     <t>project list test</t>
   </si>
   <si>
-    <t>test_sign_out</t>
-  </si>
-  <si>
     <t>login page</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>test_forgot_password_link</t>
   </si>
   <si>
-    <t>test_unsuccessful_login</t>
-  </si>
-  <si>
     <t>Check if 'Forgot Password' link works</t>
   </si>
   <si>
@@ -132,7 +126,13 @@
     <t>Check if a new user can be successfully signed up</t>
   </si>
   <si>
-    <t>test_project_list_views</t>
+    <t>test_switching_project_list_views</t>
+  </si>
+  <si>
+    <t>test_signing _out</t>
+  </si>
+  <si>
+    <t>test_preventing_unsuccessful_login_attempts</t>
   </si>
 </sst>
 </file>
@@ -506,10 +506,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A2:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +550,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -560,7 +561,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -569,7 +570,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -577,10 +578,10 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" t="s">
         <v>9</v>
@@ -589,7 +590,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -597,10 +598,10 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
@@ -611,16 +612,16 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>
@@ -631,16 +632,16 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
       <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
         <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -651,16 +652,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
       <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>29</v>
       </c>
       <c r="F8" t="s">
         <v>9</v>
@@ -671,16 +672,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
       <c r="C9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
         <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -691,16 +692,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F10" t="s">
         <v>8</v>
@@ -710,7 +711,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H10"/>
+  <autoFilter ref="A2:H10">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="login page"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>

</xml_diff>

<commit_message>
add some more utilities and test cases
</commit_message>
<xml_diff>
--- a/data_sheets/test_coverage.xlsx
+++ b/data_sheets/test_coverage.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">test_cases!$A$2:$H$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">test_cases!$A$2:$H$11</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
   <si>
     <t>PAGE</t>
   </si>
@@ -133,6 +133,18 @@
   </si>
   <si>
     <t>test_preventing_unsuccessful_login_attempts</t>
+  </si>
+  <si>
+    <t>profile page</t>
+  </si>
+  <si>
+    <t>profile page test</t>
+  </si>
+  <si>
+    <t>Editing the profile</t>
+  </si>
+  <si>
+    <t>test_changing_profile</t>
   </si>
 </sst>
 </file>
@@ -506,11 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A2:H10"/>
+  <dimension ref="A2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +561,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -570,7 +581,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -590,7 +601,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -710,30 +721,56 @@
         <v>11</v>
       </c>
     </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:H10">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="login page"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A2:H11"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!$A$3:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F21</xm:sqref>
+          <xm:sqref>F3:F10 F12:F21</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Test case completed?" prompt="Test cases has been added in the automation test suite and ready to run">
           <x14:formula1>
             <xm:f>Sheet2!$B$3:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G21</xm:sqref>
+          <xm:sqref>G3:G10 G12:G21</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Sheet2!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>F11</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Test case completed?" prompt="Test cases has been added in the automation test suite and ready to run">
+          <x14:formula1>
+            <xm:f>Sheet2!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>G11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
combine forgot_password and sign_up links on the login page to one test case -> test_links
</commit_message>
<xml_diff>
--- a/data_sheets/test_coverage.xlsx
+++ b/data_sheets/test_coverage.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">test_cases!$A$2:$H$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">test_cases!$A$2:$H$10</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
   <si>
     <t>PAGE</t>
   </si>
@@ -102,18 +102,6 @@
     <t xml:space="preserve">Switching from grid view to list view </t>
   </si>
   <si>
-    <t>test_sign_up_link</t>
-  </si>
-  <si>
-    <t>Check if sign up link works</t>
-  </si>
-  <si>
-    <t>test_forgot_password_link</t>
-  </si>
-  <si>
-    <t>Check if 'Forgot Password' link works</t>
-  </si>
-  <si>
     <t>Check if invalid login attempts are prevented</t>
   </si>
   <si>
@@ -145,6 +133,12 @@
   </si>
   <si>
     <t>test_changing_profile</t>
+  </si>
+  <si>
+    <t>test_page_links</t>
+  </si>
+  <si>
+    <t>Check if all page links are working</t>
   </si>
 </sst>
 </file>
@@ -518,10 +512,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H11"/>
+  <dimension ref="A2:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,7 +566,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -589,7 +583,7 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
@@ -609,7 +603,7 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
         <v>22</v>
@@ -649,10 +643,10 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -669,13 +663,13 @@
         <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -689,10 +683,10 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
         <v>8</v>
@@ -703,46 +697,26 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H11"/>
+  <autoFilter ref="A2:H10"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
@@ -752,25 +726,25 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$3:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F10 F12:F21</xm:sqref>
+          <xm:sqref>F11:F20 F3:F9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Test case completed?" prompt="Test cases has been added in the automation test suite and ready to run">
           <x14:formula1>
             <xm:f>Sheet2!$B$3:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G10 G12:G21</xm:sqref>
+          <xm:sqref>G11:G20 G3:G9</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Sheet2!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>F11</xm:sqref>
+          <xm:sqref>F10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Test case completed?" prompt="Test cases has been added in the automation test suite and ready to run">
           <x14:formula1>
             <xm:f>Sheet2!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>G11</xm:sqref>
+          <xm:sqref>G10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
add some modifications to the tutorial pages
</commit_message>
<xml_diff>
--- a/data_sheets/test_coverage.xlsx
+++ b/data_sheets/test_coverage.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
   <si>
     <t>PAGE</t>
   </si>
@@ -121,18 +121,6 @@
   </si>
   <si>
     <t>test_preventing_unsuccessful_login_attempts</t>
-  </si>
-  <si>
-    <t>profile page</t>
-  </si>
-  <si>
-    <t>profile page test</t>
-  </si>
-  <si>
-    <t>Editing the profile</t>
-  </si>
-  <si>
-    <t>test_changing_profile</t>
   </si>
   <si>
     <t>test_page_links</t>
@@ -512,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H10"/>
+  <dimension ref="A2:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A10" sqref="A10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,10 +631,10 @@
         <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F7" t="s">
         <v>8</v>
@@ -693,26 +681,6 @@
       </c>
       <c r="G9" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>